<commit_message>
SCRA Dec 3 25 01
</commit_message>
<xml_diff>
--- a/scra/scra_pymt_history_from_2021.xlsx
+++ b/scra/scra_pymt_history_from_2021.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="197">
   <si>
     <t>S No</t>
   </si>
@@ -757,6 +757,19 @@
   </si>
   <si>
     <t>2B Rathna Apartment, S Daniel</t>
+  </si>
+  <si>
+    <t>Akshay Apartment</t>
+  </si>
+  <si>
+    <t>N Ravichandran
+Chandra Electricals</t>
+  </si>
+  <si>
+    <t>Sadhika Shankar Rao</t>
+  </si>
+  <si>
+    <t>M Saravanan</t>
   </si>
 </sst>
 </file>
@@ -829,7 +842,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -918,6 +931,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor rgb="FFC2E0AE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1034,12 +1053,7 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1049,6 +1063,13 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1338,7 +1359,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomRight" activeCell="K54" sqref="K54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1612,7 +1633,7 @@
       <c r="J7" s="8">
         <v>1500</v>
       </c>
-      <c r="K7" s="50" t="s">
+      <c r="K7" s="49" t="s">
         <v>173</v>
       </c>
       <c r="L7" s="10"/>
@@ -1804,8 +1825,8 @@
       <c r="I12" s="8">
         <v>2500</v>
       </c>
-      <c r="J12" s="20">
-        <v>0</v>
+      <c r="J12" s="8">
+        <v>2500</v>
       </c>
       <c r="K12" s="24" t="s">
         <v>170</v>
@@ -1897,14 +1918,14 @@
       <c r="P14" s="12"/>
     </row>
     <row r="15" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="54">
+      <c r="A15" s="51">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15" s="55" t="s">
+      <c r="B15" s="52" t="s">
         <v>190</v>
       </c>
-      <c r="C15" s="55" t="s">
+      <c r="C15" s="52" t="s">
         <v>188</v>
       </c>
       <c r="D15" s="48" t="s">
@@ -1936,14 +1957,14 @@
       <c r="P15" s="12"/>
     </row>
     <row r="16" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="54">
+      <c r="A16" s="51">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B16" s="55" t="s">
+      <c r="B16" s="52" t="s">
         <v>189</v>
       </c>
-      <c r="C16" s="55" t="s">
+      <c r="C16" s="52" t="s">
         <v>188</v>
       </c>
       <c r="D16" s="48" t="s">
@@ -1967,14 +1988,14 @@
       <c r="P16" s="12"/>
     </row>
     <row r="17" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="54">
+      <c r="A17" s="51">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B17" s="55" t="s">
+      <c r="B17" s="52" t="s">
         <v>191</v>
       </c>
-      <c r="C17" s="55" t="s">
+      <c r="C17" s="52" t="s">
         <v>188</v>
       </c>
       <c r="D17" s="48" t="s">
@@ -2080,10 +2101,10 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B20" s="55" t="s">
+      <c r="B20" s="52" t="s">
         <v>192</v>
       </c>
-      <c r="C20" s="55" t="s">
+      <c r="C20" s="52" t="s">
         <v>188</v>
       </c>
       <c r="D20" s="48" t="s">
@@ -2099,7 +2120,7 @@
       <c r="J20" s="8">
         <v>1500</v>
       </c>
-      <c r="K20" s="53"/>
+      <c r="K20" s="50"/>
       <c r="L20" s="10"/>
       <c r="M20" s="11"/>
       <c r="N20" s="11"/>
@@ -2459,23 +2480,27 @@
       <c r="O29" s="11"/>
       <c r="P29" s="12"/>
     </row>
-    <row r="30" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="39">
+    <row r="30" spans="1:16" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="47">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B30" s="40" t="s">
-        <v>160</v>
-      </c>
-      <c r="C30" s="40"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="42"/>
-      <c r="J30" s="42"/>
-      <c r="K30" s="42"/>
+      <c r="B30" s="52" t="s">
+        <v>193</v>
+      </c>
+      <c r="C30" s="52" t="s">
+        <v>194</v>
+      </c>
+      <c r="D30" s="48"/>
+      <c r="E30" s="48"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9">
+        <v>7500</v>
+      </c>
+      <c r="K30" s="9"/>
       <c r="L30" s="10"/>
       <c r="M30" s="11"/>
       <c r="N30" s="11"/>
@@ -3290,8 +3315,8 @@
       <c r="I52" s="20">
         <v>0</v>
       </c>
-      <c r="J52" s="20">
-        <v>0</v>
+      <c r="J52" s="8">
+        <v>2500</v>
       </c>
       <c r="K52" s="24"/>
       <c r="L52" s="10"/>
@@ -3329,8 +3354,8 @@
       <c r="I53" s="8">
         <v>2500</v>
       </c>
-      <c r="J53" s="20">
-        <v>0</v>
+      <c r="J53" s="8">
+        <v>2500</v>
       </c>
       <c r="K53" s="24"/>
       <c r="L53" s="10"/>
@@ -3787,7 +3812,7 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
-        <f t="shared" ref="A67:A96" si="2">A66+1</f>
+        <f t="shared" ref="A67:A99" si="2">A66+1</f>
         <v>66</v>
       </c>
       <c r="B67" s="6" t="s">
@@ -3924,54 +3949,70 @@
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="39">
+      <c r="A71" s="5">
         <f t="shared" si="2"/>
         <v>70</v>
       </c>
-      <c r="B71" s="40" t="s">
-        <v>160</v>
-      </c>
-      <c r="C71" s="40"/>
-      <c r="D71" s="41"/>
-      <c r="E71" s="41"/>
-      <c r="F71" s="38"/>
-      <c r="G71" s="38"/>
-      <c r="H71" s="49"/>
-      <c r="I71" s="49"/>
-      <c r="J71" s="49"/>
-      <c r="K71" s="42"/>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B71" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D71" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F71" s="16">
+        <v>10000</v>
+      </c>
+      <c r="G71" s="19">
+        <v>0</v>
+      </c>
+      <c r="H71" s="18">
+        <v>10000</v>
+      </c>
+      <c r="I71" s="18">
+        <v>10000</v>
+      </c>
+      <c r="J71" s="18">
+        <v>10000</v>
+      </c>
+      <c r="K71" s="9"/>
+    </row>
+    <row r="72" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <f t="shared" si="2"/>
         <v>71</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D72" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F72" s="16">
+        <v>103</v>
+      </c>
+      <c r="F72" s="8">
         <v>10000</v>
       </c>
-      <c r="G72" s="19">
-        <v>0</v>
-      </c>
-      <c r="H72" s="18">
-        <v>10000</v>
-      </c>
-      <c r="I72" s="18">
-        <v>10000</v>
-      </c>
-      <c r="J72" s="18">
-        <v>10000</v>
+      <c r="G72" s="20">
+        <v>0</v>
+      </c>
+      <c r="H72" s="35">
+        <v>0</v>
+      </c>
+      <c r="I72" s="35">
+        <v>0</v>
+      </c>
+      <c r="J72" s="9">
+        <v>1500</v>
       </c>
       <c r="K72" s="9"/>
     </row>
@@ -3981,7 +4022,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>18</v>
+        <v>195</v>
       </c>
       <c r="C73" s="6" t="s">
         <v>19</v>
@@ -3990,22 +4031,14 @@
         <v>11</v>
       </c>
       <c r="E73" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F73" s="8">
-        <v>10000</v>
-      </c>
-      <c r="G73" s="20">
-        <v>0</v>
-      </c>
-      <c r="H73" s="35">
-        <v>0</v>
-      </c>
-      <c r="I73" s="35">
-        <v>0</v>
-      </c>
-      <c r="J73" s="35">
-        <v>0</v>
+        <v>103</v>
+      </c>
+      <c r="F73" s="8"/>
+      <c r="G73" s="20"/>
+      <c r="H73" s="35"/>
+      <c r="I73" s="35"/>
+      <c r="J73" s="9">
+        <v>1500</v>
       </c>
       <c r="K73" s="9"/>
     </row>
@@ -4212,7 +4245,7 @@
       <c r="K79" s="9"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A80" s="39">
+      <c r="A80" s="5">
         <f t="shared" si="2"/>
         <v>79</v>
       </c>
@@ -4230,7 +4263,7 @@
       <c r="K80" s="42"/>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A81" s="39">
+      <c r="A81" s="5">
         <f t="shared" si="2"/>
         <v>80</v>
       </c>
@@ -4262,7 +4295,7 @@
       <c r="K81" s="42"/>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A82" s="39">
+      <c r="A82" s="5">
         <f t="shared" si="2"/>
         <v>81</v>
       </c>
@@ -4319,7 +4352,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>76</v>
+        <v>196</v>
       </c>
       <c r="C84" s="6" t="s">
         <v>141</v>
@@ -4338,8 +4371,8 @@
       <c r="I84" s="9">
         <v>2500</v>
       </c>
-      <c r="J84" s="35">
-        <v>0</v>
+      <c r="J84" s="9">
+        <v>2500</v>
       </c>
       <c r="K84" s="9" t="s">
         <v>146</v>
@@ -4548,8 +4581,8 @@
       <c r="I90" s="22">
         <v>7500</v>
       </c>
-      <c r="J90" s="20">
-        <v>0</v>
+      <c r="J90" s="8">
+        <v>7500</v>
       </c>
       <c r="K90" s="24"/>
     </row>
@@ -4710,35 +4743,35 @@
       <c r="I95" s="8">
         <v>1500</v>
       </c>
-      <c r="J95" s="20">
-        <v>0</v>
+      <c r="J95" s="8">
+        <v>1500</v>
       </c>
       <c r="K95" s="8"/>
     </row>
     <row r="96" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="51">
+      <c r="A96" s="5">
         <f t="shared" si="2"/>
         <v>95</v>
       </c>
-      <c r="B96" s="52" t="s">
+      <c r="B96" s="53" t="s">
         <v>184</v>
       </c>
-      <c r="C96" s="53" t="s">
+      <c r="C96" s="54" t="s">
         <v>185</v>
       </c>
-      <c r="D96" s="51" t="s">
+      <c r="D96" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="E96" s="51" t="s">
-        <v>12</v>
-      </c>
-      <c r="F96" s="16" t="s">
+      <c r="E96" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="F96" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="G96" s="16" t="s">
+      <c r="G96" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="H96" s="16" t="s">
+      <c r="H96" s="17" t="s">
         <v>161</v>
       </c>
       <c r="I96" s="16">
@@ -4751,6 +4784,7 @@
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="5">
+        <f t="shared" si="2"/>
         <v>96</v>
       </c>
       <c r="B97" s="15" t="s">
@@ -4782,6 +4816,7 @@
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="5">
+        <f t="shared" si="2"/>
         <v>97</v>
       </c>
       <c r="B98" s="15" t="s">
@@ -4810,7 +4845,10 @@
       <c r="K98" s="9"/>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A99" s="5"/>
+      <c r="A99" s="5">
+        <f t="shared" si="2"/>
+        <v>98</v>
+      </c>
       <c r="B99" s="15"/>
       <c r="C99" s="6"/>
       <c r="D99" s="48"/>
@@ -4867,7 +4905,7 @@
       </c>
       <c r="J103" s="32">
         <f>COUNTIFS(E2:E98, "House", J2:J98, "&lt;&gt;0")</f>
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="104" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
@@ -4877,7 +4915,7 @@
       </c>
       <c r="F104" s="32">
         <f>COUNTIFS(E2:E98, "Apartment", F2:F98, "&lt;&gt;0")</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G104" s="32">
         <f>COUNTIFS(E2:E98, "Apartment", G2:G98, "&lt;&gt;0")</f>
@@ -4893,7 +4931,7 @@
       </c>
       <c r="J104" s="32">
         <f>COUNTIFS(E2:E98, "Apartment", J2:J98, "&lt;&gt;0")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="105" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
@@ -4903,23 +4941,23 @@
       </c>
       <c r="F105" s="32">
         <f>COUNTIFS(E2:E98, "Ind. Apartment", F2:F98, "&lt;&gt;0")</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G105" s="32">
         <f>COUNTIFS(E2:E98, "Ind. Apartment", G2:G98, "&lt;&gt;0.00")</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H105" s="32">
         <f>COUNTIFS(E2:E98, "Ind. Apartment", H2:H98, "&lt;&gt;0")</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I105" s="32">
         <f>COUNTIFS(E2:E98, "Ind. Apartment", I2:I98, "&lt;&gt;0")</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J105" s="32">
         <f>COUNTIFS(E2:E98, "Ind. Apartment", J2:J98, "&lt;&gt;0")</f>
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="106" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
@@ -4963,7 +5001,7 @@
       </c>
       <c r="J110" s="32">
         <f>COUNTIFS(D2:D98, "1st Main", J2:J98, "&lt;&gt;0")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="111" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
@@ -5013,7 +5051,7 @@
       </c>
       <c r="J112" s="32">
         <f>COUNTIFS(D2:D98, "3rd Main", J2:J98, "&lt;&gt;0")</f>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="113" spans="5:10" ht="18.75" x14ac:dyDescent="0.3">
@@ -5122,23 +5160,23 @@
       </c>
       <c r="F117" s="32">
         <f>COUNTIFS(D2:D98, "Seethammal Road", F2:F98, "&lt;&gt;0")</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G117" s="32">
         <f>COUNTIFS(D2:D98, "Seethammal Road", G2:G98, "&lt;&gt;0")</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H117" s="32">
         <f>COUNTIFS(D2:D98, "Seethammal Road", H2:H98, "&lt;&gt;0")</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I117" s="32">
         <f>COUNTIFS(D2:D98, "Seethammal Road", I2:I98, "&lt;&gt;0")</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J117" s="32">
         <f>COUNTIFS(D2:D98, "Seethammal Road", J2:J98, "&lt;&gt;0")</f>
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>